<commit_message>
JL 1 person added
1 person added as a test
</commit_message>
<xml_diff>
--- a/Patient details.xlsx
+++ b/Patient details.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\conor_000\Documents\a.SD\GitHub\Software-Testing-And-Verification\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonnie\Documents\Software Development\CSC7051 Programming II\Group Project\Programming-II\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="912" uniqueCount="503">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="914" uniqueCount="505">
   <si>
     <t>NHS Number</t>
   </si>
@@ -1528,6 +1528,12 @@
   </si>
   <si>
     <t>Morrison</t>
+  </si>
+  <si>
+    <t>Margot</t>
+  </si>
+  <si>
+    <t>Robbie</t>
   </si>
 </sst>
 </file>
@@ -1874,8 +1880,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H200"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2954,6 +2960,12 @@
       <c r="B46" t="s">
         <v>9</v>
       </c>
+      <c r="C46" t="s">
+        <v>503</v>
+      </c>
+      <c r="D46" t="s">
+        <v>504</v>
+      </c>
       <c r="E46" t="s">
         <v>275</v>
       </c>

</xml_diff>

<commit_message>
People added up to 80
Names mostly derived from The Wolf of Wall Street cast
</commit_message>
<xml_diff>
--- a/Patient details.xlsx
+++ b/Patient details.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="914" uniqueCount="505">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="982" uniqueCount="568">
   <si>
     <t>NHS Number</t>
   </si>
@@ -1534,6 +1534,195 @@
   </si>
   <si>
     <t>Robbie</t>
+  </si>
+  <si>
+    <t>Leonardo</t>
+  </si>
+  <si>
+    <t>DiCaprio</t>
+  </si>
+  <si>
+    <t>Jonah</t>
+  </si>
+  <si>
+    <t>Hill</t>
+  </si>
+  <si>
+    <t>McConaughey</t>
+  </si>
+  <si>
+    <t>Kyle</t>
+  </si>
+  <si>
+    <t>Chandler</t>
+  </si>
+  <si>
+    <t>Rob</t>
+  </si>
+  <si>
+    <t>Reiner</t>
+  </si>
+  <si>
+    <t>Jon</t>
+  </si>
+  <si>
+    <t>Bernthal</t>
+  </si>
+  <si>
+    <t>Favreau</t>
+  </si>
+  <si>
+    <t>Jean</t>
+  </si>
+  <si>
+    <t>Dujardin</t>
+  </si>
+  <si>
+    <t>Joanna</t>
+  </si>
+  <si>
+    <t>Lumley</t>
+  </si>
+  <si>
+    <t>Cristin</t>
+  </si>
+  <si>
+    <t>Milioti</t>
+  </si>
+  <si>
+    <t>Christine</t>
+  </si>
+  <si>
+    <t>Ebersole</t>
+  </si>
+  <si>
+    <t>Shea</t>
+  </si>
+  <si>
+    <t>Whigham</t>
+  </si>
+  <si>
+    <t>Katarina</t>
+  </si>
+  <si>
+    <t>Cas</t>
+  </si>
+  <si>
+    <t>Kenneth</t>
+  </si>
+  <si>
+    <t>Choi</t>
+  </si>
+  <si>
+    <t>Brian</t>
+  </si>
+  <si>
+    <t>Sacca</t>
+  </si>
+  <si>
+    <t>Henry</t>
+  </si>
+  <si>
+    <t>Zebrowski</t>
+  </si>
+  <si>
+    <t>Ethan</t>
+  </si>
+  <si>
+    <t>Suplee</t>
+  </si>
+  <si>
+    <t>Barry</t>
+  </si>
+  <si>
+    <t>Rothbart</t>
+  </si>
+  <si>
+    <t>Megan</t>
+  </si>
+  <si>
+    <t>McKenzie</t>
+  </si>
+  <si>
+    <t>Hoffman</t>
+  </si>
+  <si>
+    <t>Amy</t>
+  </si>
+  <si>
+    <t>Cash</t>
+  </si>
+  <si>
+    <t>Stephanie</t>
+  </si>
+  <si>
+    <t>McCoy</t>
+  </si>
+  <si>
+    <t>Ashley</t>
+  </si>
+  <si>
+    <t>Atkinson</t>
+  </si>
+  <si>
+    <t>Ted</t>
+  </si>
+  <si>
+    <t>Griffin</t>
+  </si>
+  <si>
+    <t>Edward</t>
+  </si>
+  <si>
+    <t>Hermann</t>
+  </si>
+  <si>
+    <t>Stephen</t>
+  </si>
+  <si>
+    <t>O'Neill</t>
+  </si>
+  <si>
+    <t>Natasha</t>
+  </si>
+  <si>
+    <t>Thomas</t>
+  </si>
+  <si>
+    <t>Sandra</t>
+  </si>
+  <si>
+    <t>Nelson</t>
+  </si>
+  <si>
+    <t>Carla</t>
+  </si>
+  <si>
+    <t>Flaherty</t>
+  </si>
+  <si>
+    <t>Madison</t>
+  </si>
+  <si>
+    <t>McKinley</t>
+  </si>
+  <si>
+    <t>Diedre</t>
+  </si>
+  <si>
+    <t>Reimond</t>
+  </si>
+  <si>
+    <t>Malloy</t>
+  </si>
+  <si>
+    <t>Witting</t>
+  </si>
+  <si>
+    <t>Tess</t>
+  </si>
+  <si>
+    <t>Gillis</t>
   </si>
 </sst>
 </file>
@@ -1880,8 +2069,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H200"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="D46" sqref="D46"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2984,6 +3173,12 @@
       <c r="B47" t="s">
         <v>11</v>
       </c>
+      <c r="C47" t="s">
+        <v>505</v>
+      </c>
+      <c r="D47" t="s">
+        <v>506</v>
+      </c>
       <c r="E47" t="s">
         <v>312</v>
       </c>
@@ -3001,6 +3196,12 @@
       <c r="B48" t="s">
         <v>8</v>
       </c>
+      <c r="C48" t="s">
+        <v>507</v>
+      </c>
+      <c r="D48" t="s">
+        <v>508</v>
+      </c>
       <c r="E48" t="s">
         <v>439</v>
       </c>
@@ -3018,6 +3219,12 @@
       <c r="B49" t="s">
         <v>11</v>
       </c>
+      <c r="C49" t="s">
+        <v>457</v>
+      </c>
+      <c r="D49" t="s">
+        <v>509</v>
+      </c>
       <c r="E49" t="s">
         <v>311</v>
       </c>
@@ -3036,6 +3243,12 @@
       <c r="B50" t="s">
         <v>10</v>
       </c>
+      <c r="C50" t="s">
+        <v>527</v>
+      </c>
+      <c r="D50" t="s">
+        <v>528</v>
+      </c>
       <c r="E50" t="s">
         <v>447</v>
       </c>
@@ -3053,6 +3266,12 @@
       <c r="B51" t="s">
         <v>10</v>
       </c>
+      <c r="C51" t="s">
+        <v>562</v>
+      </c>
+      <c r="D51" t="s">
+        <v>563</v>
+      </c>
       <c r="E51" t="s">
         <v>68</v>
       </c>
@@ -3070,6 +3289,12 @@
       <c r="B52" t="s">
         <v>9</v>
       </c>
+      <c r="C52" t="s">
+        <v>494</v>
+      </c>
+      <c r="D52" t="s">
+        <v>564</v>
+      </c>
       <c r="E52" t="s">
         <v>431</v>
       </c>
@@ -3087,6 +3312,12 @@
       <c r="B53" t="s">
         <v>10</v>
       </c>
+      <c r="C53" t="s">
+        <v>544</v>
+      </c>
+      <c r="D53" t="s">
+        <v>565</v>
+      </c>
       <c r="E53" t="s">
         <v>388</v>
       </c>
@@ -3104,6 +3335,12 @@
       <c r="B54" t="s">
         <v>9</v>
       </c>
+      <c r="C54" t="s">
+        <v>566</v>
+      </c>
+      <c r="D54" t="s">
+        <v>567</v>
+      </c>
       <c r="E54" t="s">
         <v>375</v>
       </c>
@@ -3122,6 +3359,12 @@
       <c r="B55" t="s">
         <v>10</v>
       </c>
+      <c r="C55" t="s">
+        <v>523</v>
+      </c>
+      <c r="D55" t="s">
+        <v>524</v>
+      </c>
       <c r="E55" t="s">
         <v>413</v>
       </c>
@@ -3140,6 +3383,12 @@
       <c r="B56" t="s">
         <v>8</v>
       </c>
+      <c r="C56" t="s">
+        <v>510</v>
+      </c>
+      <c r="D56" t="s">
+        <v>511</v>
+      </c>
       <c r="E56" t="s">
         <v>59</v>
       </c>
@@ -3157,6 +3406,12 @@
       <c r="B57" t="s">
         <v>8</v>
       </c>
+      <c r="C57" t="s">
+        <v>512</v>
+      </c>
+      <c r="D57" t="s">
+        <v>513</v>
+      </c>
       <c r="E57" t="s">
         <v>306</v>
       </c>
@@ -3174,6 +3429,12 @@
       <c r="B58" t="s">
         <v>9</v>
       </c>
+      <c r="C58" t="s">
+        <v>521</v>
+      </c>
+      <c r="D58" t="s">
+        <v>522</v>
+      </c>
       <c r="E58" t="s">
         <v>444</v>
       </c>
@@ -3194,6 +3455,12 @@
       <c r="B59" t="s">
         <v>8</v>
       </c>
+      <c r="C59" t="s">
+        <v>514</v>
+      </c>
+      <c r="D59" t="s">
+        <v>515</v>
+      </c>
       <c r="E59" t="s">
         <v>64</v>
       </c>
@@ -3214,6 +3481,12 @@
       <c r="B60" t="s">
         <v>10</v>
       </c>
+      <c r="C60" t="s">
+        <v>519</v>
+      </c>
+      <c r="D60" t="s">
+        <v>520</v>
+      </c>
       <c r="E60" t="s">
         <v>316</v>
       </c>
@@ -3231,6 +3504,12 @@
       <c r="B61" t="s">
         <v>8</v>
       </c>
+      <c r="C61" t="s">
+        <v>514</v>
+      </c>
+      <c r="D61" t="s">
+        <v>516</v>
+      </c>
       <c r="E61" t="s">
         <v>303</v>
       </c>
@@ -3249,6 +3528,12 @@
       <c r="B62" t="s">
         <v>8</v>
       </c>
+      <c r="C62" t="s">
+        <v>517</v>
+      </c>
+      <c r="D62" t="s">
+        <v>518</v>
+      </c>
       <c r="E62" t="s">
         <v>367</v>
       </c>
@@ -3266,6 +3551,12 @@
       <c r="B63" t="s">
         <v>9</v>
       </c>
+      <c r="C63" t="s">
+        <v>539</v>
+      </c>
+      <c r="D63" t="s">
+        <v>540</v>
+      </c>
       <c r="E63" t="s">
         <v>71</v>
       </c>
@@ -3283,6 +3574,12 @@
       <c r="B64" t="s">
         <v>9</v>
       </c>
+      <c r="C64" t="s">
+        <v>542</v>
+      </c>
+      <c r="D64" t="s">
+        <v>543</v>
+      </c>
       <c r="E64" t="s">
         <v>339</v>
       </c>
@@ -3300,6 +3597,12 @@
       <c r="B65" t="s">
         <v>9</v>
       </c>
+      <c r="C65" t="s">
+        <v>544</v>
+      </c>
+      <c r="D65" t="s">
+        <v>545</v>
+      </c>
       <c r="E65" t="s">
         <v>60</v>
       </c>
@@ -3317,6 +3620,12 @@
       <c r="B66" t="s">
         <v>8</v>
       </c>
+      <c r="C66" t="s">
+        <v>525</v>
+      </c>
+      <c r="D66" t="s">
+        <v>526</v>
+      </c>
       <c r="E66" t="s">
         <v>307</v>
       </c>
@@ -3334,6 +3643,12 @@
       <c r="B67" t="s">
         <v>10</v>
       </c>
+      <c r="C67" t="s">
+        <v>560</v>
+      </c>
+      <c r="D67" t="s">
+        <v>561</v>
+      </c>
       <c r="E67" t="s">
         <v>276</v>
       </c>
@@ -3351,6 +3666,12 @@
       <c r="B68" t="s">
         <v>8</v>
       </c>
+      <c r="C68" t="s">
+        <v>529</v>
+      </c>
+      <c r="D68" t="s">
+        <v>530</v>
+      </c>
       <c r="E68" t="s">
         <v>282</v>
       </c>
@@ -3371,6 +3692,12 @@
       <c r="B69" t="s">
         <v>8</v>
       </c>
+      <c r="C69" t="s">
+        <v>531</v>
+      </c>
+      <c r="D69" t="s">
+        <v>532</v>
+      </c>
       <c r="E69" t="s">
         <v>428</v>
       </c>
@@ -3388,6 +3715,12 @@
       <c r="B70" t="s">
         <v>8</v>
       </c>
+      <c r="C70" t="s">
+        <v>533</v>
+      </c>
+      <c r="D70" t="s">
+        <v>534</v>
+      </c>
       <c r="E70" t="s">
         <v>393</v>
       </c>
@@ -3405,6 +3738,12 @@
       <c r="B71" t="s">
         <v>9</v>
       </c>
+      <c r="C71" t="s">
+        <v>546</v>
+      </c>
+      <c r="D71" t="s">
+        <v>547</v>
+      </c>
       <c r="E71" t="s">
         <v>412</v>
       </c>
@@ -3422,6 +3761,12 @@
       <c r="B72" t="s">
         <v>10</v>
       </c>
+      <c r="C72" t="s">
+        <v>558</v>
+      </c>
+      <c r="D72" t="s">
+        <v>559</v>
+      </c>
       <c r="E72" t="s">
         <v>294</v>
       </c>
@@ -3439,6 +3784,12 @@
       <c r="B73" t="s">
         <v>8</v>
       </c>
+      <c r="C73" t="s">
+        <v>535</v>
+      </c>
+      <c r="D73" t="s">
+        <v>536</v>
+      </c>
       <c r="E73" t="s">
         <v>416</v>
       </c>
@@ -3456,6 +3807,12 @@
       <c r="B74" t="s">
         <v>8</v>
       </c>
+      <c r="C74" t="s">
+        <v>537</v>
+      </c>
+      <c r="D74" t="s">
+        <v>538</v>
+      </c>
       <c r="E74" t="s">
         <v>315</v>
       </c>
@@ -3476,6 +3833,12 @@
       <c r="B75" t="s">
         <v>9</v>
       </c>
+      <c r="C75" t="s">
+        <v>556</v>
+      </c>
+      <c r="D75" t="s">
+        <v>557</v>
+      </c>
       <c r="E75" t="s">
         <v>390</v>
       </c>
@@ -3493,6 +3856,12 @@
       <c r="B76" t="s">
         <v>9</v>
       </c>
+      <c r="C76" t="s">
+        <v>554</v>
+      </c>
+      <c r="D76" t="s">
+        <v>555</v>
+      </c>
       <c r="E76" t="s">
         <v>281</v>
       </c>
@@ -3510,6 +3879,12 @@
       <c r="B77" t="s">
         <v>8</v>
       </c>
+      <c r="C77" t="s">
+        <v>479</v>
+      </c>
+      <c r="D77" t="s">
+        <v>541</v>
+      </c>
       <c r="E77" t="s">
         <v>391</v>
       </c>
@@ -3527,6 +3902,12 @@
       <c r="B78" t="s">
         <v>8</v>
       </c>
+      <c r="C78" t="s">
+        <v>552</v>
+      </c>
+      <c r="D78" t="s">
+        <v>553</v>
+      </c>
       <c r="E78" t="s">
         <v>309</v>
       </c>
@@ -3545,6 +3926,12 @@
       <c r="B79" t="s">
         <v>8</v>
       </c>
+      <c r="C79" t="s">
+        <v>550</v>
+      </c>
+      <c r="D79" t="s">
+        <v>551</v>
+      </c>
       <c r="E79" t="s">
         <v>365</v>
       </c>
@@ -3561,6 +3948,12 @@
       </c>
       <c r="B80" t="s">
         <v>8</v>
+      </c>
+      <c r="C80" t="s">
+        <v>548</v>
+      </c>
+      <c r="D80" t="s">
+        <v>549</v>
       </c>
       <c r="E80" t="s">
         <v>403</v>

</xml_diff>